<commit_message>
Updated .gitignore with macOS system files and created first version of convert tool.
</commit_message>
<xml_diff>
--- a/tests/data/testfile.xlsx
+++ b/tests/data/testfile.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,15 +20,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">potato</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> kartoffel</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> patate</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">uuid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">untested</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selenium, click</t>
+  </si>
+  <si>
+    <t xml:space="preserve">para1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selenium, write</t>
+  </si>
+  <si>
+    <t xml:space="preserve">para2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">para3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">para4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click next</t>
+  </si>
+  <si>
+    <t xml:space="preserve">para5</t>
   </si>
 </sst>
 </file>
@@ -43,6 +103,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -124,61 +185,119 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="0" t="n">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>9</v>
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>